<commit_message>
bug fix in scale gblems_expanded
</commit_message>
<xml_diff>
--- a/gblems_expanded.xlsx
+++ b/gblems_expanded.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantracy/Desktop/andre rc studies/police meta perceptions project/study 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantracy/Desktop/andre rc studies/police meta perceptions project/study 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15DF996-2311-9E49-9910-D57CC4E72996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23901D0-847A-F548-A9B7-FF751F9CB507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4060" yWindow="3160" windowWidth="27240" windowHeight="16440" xr2:uid="{41654286-75BC-2243-9840-52009D08B340}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>domain</t>
   </si>
@@ -452,7 +452,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="C4" sqref="C3:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,6 +492,12 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">

</xml_diff>